<commit_message>
delete example run files
</commit_message>
<xml_diff>
--- a/example/results_example.xlsx
+++ b/example/results_example.xlsx
@@ -556,46 +556,46 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <v>124783</v>
+        <v>128535.12</v>
       </c>
       <c r="C2">
-        <v>87348.10000000001</v>
+        <v>89974.58</v>
       </c>
       <c r="D2">
-        <v>37434.9</v>
+        <v>38560.54</v>
       </c>
       <c r="E2">
-        <v>83394.28</v>
+        <v>85905.53</v>
       </c>
       <c r="F2">
-        <v>5531.83</v>
+        <v>5694.52</v>
       </c>
       <c r="G2">
-        <v>66506.17</v>
+        <v>68505.96000000001</v>
       </c>
       <c r="H2">
-        <v>389.84</v>
+        <v>401.57</v>
       </c>
       <c r="I2">
-        <v>93.16</v>
+        <v>95.95999999999999</v>
       </c>
       <c r="J2">
-        <v>72212.44</v>
+        <v>74368.59</v>
       </c>
       <c r="K2">
-        <v>71076.03</v>
+        <v>73139.78999999999</v>
       </c>
       <c r="L2">
-        <v>71251.59</v>
+        <v>73414.06</v>
       </c>
       <c r="M2">
-        <v>144076.02</v>
+        <v>148400.96</v>
       </c>
       <c r="N2">
-        <v>21279.07</v>
+        <v>21918.92</v>
       </c>
       <c r="O2">
-        <v>5849.64</v>
+        <v>6025.53</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -650,10 +650,10 @@
         <v>1.050695888108961</v>
       </c>
       <c r="E4">
-        <v>1.012667421292953</v>
+        <v>1.012667396236561</v>
       </c>
       <c r="F4">
-        <v>1.157060235648466</v>
+        <v>1.157060676825656</v>
       </c>
       <c r="G4">
         <v>1.033566887404825</v>
@@ -665,13 +665,13 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <v>1.002251395497425</v>
+        <v>1.002101752710336</v>
       </c>
       <c r="K4">
-        <v>1.000489686985356</v>
+        <v>1.000393627332655</v>
       </c>
       <c r="L4">
-        <v>1.034220927754378</v>
+        <v>1.034459229562604</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -741,10 +741,10 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>4.53779622790608</v>
+        <v>4.409754900570112</v>
       </c>
       <c r="L8">
-        <v>17.85927280835378</v>
+        <v>17.98259849983794</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -758,7 +758,7 @@
         <v>15.3857</v>
       </c>
       <c r="D9">
-        <v>36.33336666666668</v>
+        <v>36.33336666666666</v>
       </c>
       <c r="E9">
         <v>12.1331279945243</v>
@@ -776,13 +776,13 @@
         <v>0</v>
       </c>
       <c r="J9">
-        <v>6.887635214827924</v>
+        <v>6.687943893034388</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>25.16130129998028</v>
+        <v>25.35213050123805</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -799,13 +799,13 @@
         <v>0.6705</v>
       </c>
       <c r="E10">
-        <v>0.6049965531745645</v>
+        <v>0.6049708395891255</v>
       </c>
       <c r="F10">
-        <v>0.6134623338588606</v>
+        <v>0.6138556679281634</v>
       </c>
       <c r="G10">
-        <v>0.353403227352852</v>
+        <v>0.3534032273528521</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0.3774942702737736</v>
+        <v>0.3773914661224246</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -837,10 +837,10 @@
         <v>4.568466666666666</v>
       </c>
       <c r="E11">
-        <v>0.04245589846839049</v>
+        <v>0.04245409400625442</v>
       </c>
       <c r="F11">
-        <v>0.04304998834097267</v>
+        <v>0.04307759073180095</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -858,7 +858,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0.003342316732497454</v>
+        <v>0.003341406509317179</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -875,10 +875,10 @@
         <v>1.4475</v>
       </c>
       <c r="E12">
-        <v>0.03184192385129286</v>
+        <v>0.03184057050469082</v>
       </c>
       <c r="F12">
-        <v>0.03228749125572951</v>
+        <v>0.03230819304885071</v>
       </c>
       <c r="G12">
         <v>0.03571764445946476</v>
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0.03584555499335701</v>
+        <v>0.03583579306542615</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -910,13 +910,13 @@
         <v>0.06560000000000006</v>
       </c>
       <c r="D13">
-        <v>10.78026666666667</v>
+        <v>10.78026666666666</v>
       </c>
       <c r="E13">
-        <v>0.1061397461709762</v>
+        <v>0.1061352350156361</v>
       </c>
       <c r="F13">
-        <v>0.1076249708524317</v>
+        <v>0.1076939768295024</v>
       </c>
       <c r="G13">
         <v>6.26622690463195</v>
@@ -934,7 +934,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>5.857246389115486</v>
+        <v>5.85565126756877</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -950,7 +950,7 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>72.78085490033105</v>
+        <v>74.96931608889483</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>18</v>
@@ -964,7 +964,7 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>14.73886343673511</v>
+        <v>15.0270094682561</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>19</v>
@@ -978,7 +978,7 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>1423.13980291352</v>
+        <v>1448.738524629777</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
@@ -992,7 +992,7 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>703.1775429981387</v>
+        <v>703.3036818639184</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>21</v>
@@ -1019,7 +1019,7 @@
         <v>23</v>
       </c>
       <c r="B26">
-        <v>389.8435809378469</v>
+        <v>401.5658607552735</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1027,7 +1027,7 @@
         <v>24</v>
       </c>
       <c r="B27">
-        <v>93.16048499276177</v>
+        <v>95.96174510427927</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1035,7 +1035,7 @@
         <v>25</v>
       </c>
       <c r="B28">
-        <v>72514.81330646758</v>
+        <v>74670.96155344439</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1043,7 +1043,7 @@
         <v>26</v>
       </c>
       <c r="B29">
-        <v>72212.44454355756</v>
+        <v>74368.59279053439</v>
       </c>
     </row>
   </sheetData>
@@ -1086,7 +1086,7 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>-144076.0160331408</v>
+        <v>-148400.962485911</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -1114,7 +1114,7 @@
         <v>30</v>
       </c>
       <c r="B5">
-        <v>2213.837064248725</v>
+        <v>2242.038532050846</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -1142,7 +1142,7 @@
         <v>32</v>
       </c>
       <c r="B7">
-        <v>4383397.387212477</v>
+        <v>4439236.293460676</v>
       </c>
       <c r="C7" s="1">
         <v>5</v>
@@ -1156,7 +1156,7 @@
         <v>33</v>
       </c>
       <c r="B8">
-        <v>144076.0160331408</v>
+        <v>148400.962485911</v>
       </c>
       <c r="C8" s="1">
         <v>6</v>
@@ -1170,7 +1170,7 @@
         <v>34</v>
       </c>
       <c r="B9">
-        <v>3664332.219062699</v>
+        <v>3714921.257162649</v>
       </c>
       <c r="C9" s="1">
         <v>7</v>
@@ -1184,7 +1184,7 @@
         <v>35</v>
       </c>
       <c r="B10">
-        <v>5911189.337268497</v>
+        <v>6017025.973444377</v>
       </c>
       <c r="C10" s="1">
         <v>8</v>

</xml_diff>